<commit_message>
updated accounting export mapping
</commit_message>
<xml_diff>
--- a/support/export_spreadsheets/mappings/accounting_spreadsheet_mapping.xlsx
+++ b/support/export_spreadsheets/mappings/accounting_spreadsheet_mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\perry\Dropbox (Science Center)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\perry\Dropbox (Science Center)\perry\ca_mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="108">
   <si>
     <t>Rule type</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Related storage locations (Current location)</t>
   </si>
   <si>
-    <t>Owned by/loaned to</t>
-  </si>
-  <si>
     <t>Insurance value</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
     <t>Current location</t>
   </si>
   <si>
-    <t>Owned by/Loaned to</t>
-  </si>
-  <si>
     <t>ca_storage_locations.hierarchy.preferred_labels.name</t>
   </si>
   <si>
@@ -307,9 +301,6 @@
   </si>
   <si>
     <t>ExDev room 465</t>
-  </si>
-  <si>
-    <t>ca_objects.owned_by_loaned_to</t>
   </si>
   <si>
     <t>ca_objects.insurance_method</t>
@@ -356,20 +347,13 @@
     <t>export_accounting_spreadsheet</t>
   </si>
   <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>{
-    "context": "ca_entities",
-    "restrictToRelationshipTypes": ["contact"],
-    "delimiter": "; "
-}</t>
-  </si>
-  <si>
-    <t>Related entities (Contact)</t>
-  </si>
-  <si>
     <t>Accounting spreadsheet export mapping</t>
+  </si>
+  <si>
+    <t>Supergroup</t>
+  </si>
+  <si>
+    <t>ca_objects.supergroup</t>
   </si>
 </sst>
 </file>
@@ -425,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -446,6 +430,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,21 +754,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="3">
+        <v>106</v>
+      </c>
+      <c r="D2" s="11">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
+      <c r="E2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -788,56 +779,53 @@
         <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="D3" s="3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="3">
         <v>3</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>108</v>
+        <v>45</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>50</v>
+      <c r="E5" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="G5" t="s">
-        <v>110</v>
+        <v>101</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -851,7 +839,7 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
@@ -868,7 +856,7 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
         <v>28</v>
@@ -879,16 +867,16 @@
         <v>10</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D8" s="3">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -896,16 +884,16 @@
         <v>10</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="3">
         <v>8</v>
       </c>
       <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="G9" t="s">
         <v>29</v>
@@ -916,19 +904,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D10" s="3">
         <v>9</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>96</v>
+      <c r="E10" t="s">
+        <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -936,16 +921,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D11" s="3">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -958,45 +943,45 @@
       <c r="D12" s="3">
         <v>11</v>
       </c>
-      <c r="E12" t="s">
-        <v>38</v>
+      <c r="E12" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="G12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="G13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>6</v>
+      <c r="E18" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1004,16 +989,16 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1021,16 +1006,16 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>111</v>
+        <v>18</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1038,16 +1023,13 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1055,13 +1037,13 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1071,33 +1053,19 @@
       <c r="B23" t="s">
         <v>39</v>
       </c>
-      <c r="C23" t="s">
-        <v>41</v>
+      <c r="C23">
+        <v>1</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="E23" t="s">
         <v>43</v>
-      </c>
-      <c r="E24" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1118,266 +1086,266 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1385,10 +1353,10 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C25" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1396,10 +1364,10 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>